<commit_message>
updated labels and xml
</commit_message>
<xml_diff>
--- a/letters/ResetPasswordLetter/rowsForView.xlsx
+++ b/letters/ResetPasswordLetter/rowsForView.xlsx
@@ -170,16 +170,16 @@
       </c>
       <c r="C3" s="1" t="inlineStr">
         <is>
-          <t>Library Account Login with barcode</t>
+          <t>Library Account Login with Barcode</t>
         </is>
       </c>
       <c r="D3" s="1" t="inlineStr">
         <is>
-          <t>940000258</t>
+          <t>960024377</t>
         </is>
       </c>
       <c r="E3" s="2" t="n">
-        <v>44587.0</v>
+        <v>44588.0</v>
       </c>
     </row>
     <row r="4" customHeight="true" ht="15.0">
@@ -195,16 +195,16 @@
       </c>
       <c r="C4" s="1" t="inlineStr">
         <is>
-          <t>Library Account Login with barcode</t>
+          <t>Library Account Login with Barcode</t>
         </is>
       </c>
       <c r="D4" s="1" t="inlineStr">
         <is>
-          <t>940000258</t>
+          <t>960024377</t>
         </is>
       </c>
       <c r="E4" s="2" t="n">
-        <v>44587.0</v>
+        <v>44588.0</v>
       </c>
     </row>
     <row r="5" customHeight="true" ht="15.0">

</xml_diff>